<commit_message>
`chore: Update .gitignore file`
</commit_message>
<xml_diff>
--- a/test/doc/perception-belbin-feuille.xlsx
+++ b/test/doc/perception-belbin-feuille.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isafaris\Documents\Old Desktop\MES DOCUMENTS\PERSO\FORMATION\Management &amp; Leadership\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsem/Documents/code/document_translator/test/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53C160-2230-764D-A0DA-64CA14D6B0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="1" r:id="rId1"/>
     <sheet name="Résultats" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -806,7 +818,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,14 +1172,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,6 +1196,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>431800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAAB147-D38B-6C1A-2C1D-CB20A141ECE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12293600" y="9245600"/>
+          <a:ext cx="5588000" cy="7048500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6614300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>35700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>340500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>73800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253552C7-BDEA-E387-DA7F-BF286B935114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8201800" y="12049900"/>
+          <a:ext cx="3975100" cy="1587500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>604800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>122200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6345200</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95FC486D-D10C-46DD-6FC6-486482E9F902}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="922300" y="11933200"/>
+          <a:ext cx="7010400" cy="4635500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1448,32 +1615,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="68.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="68.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="40" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" ht="145" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
@@ -1484,7 +1651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1660,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1669,7 @@
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1511,7 +1678,7 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1520,7 +1687,7 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1529,7 +1696,7 @@
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1538,7 +1705,7 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1714,7 @@
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1556,7 +1723,7 @@
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1565,8 +1732,8 @@
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
@@ -1577,7 +1744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -1586,7 +1753,7 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1762,7 @@
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1604,7 +1771,7 @@
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1780,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1622,7 +1789,7 @@
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
@@ -1631,7 +1798,7 @@
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +1807,7 @@
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
@@ -1649,7 +1816,7 @@
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
@@ -1658,8 +1825,8 @@
       </c>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>33</v>
       </c>
@@ -1670,7 +1837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1679,7 +1846,7 @@
       </c>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
@@ -1688,7 +1855,7 @@
       </c>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
@@ -1697,7 +1864,7 @@
       </c>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>11</v>
       </c>
@@ -1706,7 +1873,7 @@
       </c>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
@@ -1715,7 +1882,7 @@
       </c>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
@@ -1724,7 +1891,7 @@
       </c>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>14</v>
       </c>
@@ -1733,7 +1900,7 @@
       </c>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -1742,7 +1909,7 @@
       </c>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>16</v>
       </c>
@@ -1751,8 +1918,8 @@
       </c>
       <c r="C37" s="9"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>44</v>
       </c>
@@ -1763,7 +1930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -1772,7 +1939,7 @@
       </c>
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1948,7 @@
       </c>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1957,7 @@
       </c>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>11</v>
       </c>
@@ -1799,7 +1966,7 @@
       </c>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +1975,7 @@
       </c>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>13</v>
       </c>
@@ -1817,7 +1984,7 @@
       </c>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>14</v>
       </c>
@@ -1826,7 +1993,7 @@
       </c>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>15</v>
       </c>
@@ -1835,7 +2002,7 @@
       </c>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>16</v>
       </c>
@@ -1844,8 +2011,8 @@
       </c>
       <c r="C48" s="9"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>55</v>
       </c>
@@ -1856,7 +2023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>5</v>
       </c>
@@ -1865,7 +2032,7 @@
       </c>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +2041,7 @@
       </c>
       <c r="C52" s="6"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>8</v>
       </c>
@@ -1883,7 +2050,7 @@
       </c>
       <c r="C53" s="6"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>11</v>
       </c>
@@ -1892,7 +2059,7 @@
       </c>
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +2068,7 @@
       </c>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>13</v>
       </c>
@@ -1910,7 +2077,7 @@
       </c>
       <c r="C56" s="6"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>14</v>
       </c>
@@ -1919,7 +2086,7 @@
       </c>
       <c r="C57" s="6"/>
     </row>
-    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>15</v>
       </c>
@@ -1928,7 +2095,7 @@
       </c>
       <c r="C58" s="6"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>16</v>
       </c>
@@ -1937,8 +2104,8 @@
       </c>
       <c r="C59" s="9"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>66</v>
       </c>
@@ -1949,7 +2116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +2125,7 @@
       </c>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -1967,7 +2134,7 @@
       </c>
       <c r="C63" s="6"/>
     </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>8</v>
       </c>
@@ -1976,7 +2143,7 @@
       </c>
       <c r="C64" s="6"/>
     </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>11</v>
       </c>
@@ -1985,7 +2152,7 @@
       </c>
       <c r="C65" s="6"/>
     </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>12</v>
       </c>
@@ -1994,7 +2161,7 @@
       </c>
       <c r="C66" s="6"/>
     </row>
-    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>13</v>
       </c>
@@ -2003,7 +2170,7 @@
       </c>
       <c r="C67" s="6"/>
     </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>14</v>
       </c>
@@ -2012,7 +2179,7 @@
       </c>
       <c r="C68" s="6"/>
     </row>
-    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>15</v>
       </c>
@@ -2021,7 +2188,7 @@
       </c>
       <c r="C69" s="6"/>
     </row>
-    <row r="70" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>16</v>
       </c>
@@ -2030,8 +2197,8 @@
       </c>
       <c r="C70" s="9"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
         <v>77</v>
       </c>
@@ -2042,7 +2209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>5</v>
       </c>
@@ -2051,7 +2218,7 @@
       </c>
       <c r="C73" s="6"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>6</v>
       </c>
@@ -2060,7 +2227,7 @@
       </c>
       <c r="C74" s="6"/>
     </row>
-    <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>8</v>
       </c>
@@ -2069,7 +2236,7 @@
       </c>
       <c r="C75" s="6"/>
     </row>
-    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>11</v>
       </c>
@@ -2078,7 +2245,7 @@
       </c>
       <c r="C76" s="6"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>12</v>
       </c>
@@ -2087,7 +2254,7 @@
       </c>
       <c r="C77" s="6"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>13</v>
       </c>
@@ -2096,7 +2263,7 @@
       </c>
       <c r="C78" s="6"/>
     </row>
-    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>14</v>
       </c>
@@ -2105,7 +2272,7 @@
       </c>
       <c r="C79" s="6"/>
     </row>
-    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>15</v>
       </c>
@@ -2114,7 +2281,7 @@
       </c>
       <c r="C80" s="6"/>
     </row>
-    <row r="81" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>16</v>
       </c>
@@ -2130,21 +2297,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="91.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="91.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
         <v>89</v>
       </c>
@@ -2152,9 +2319,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="24">
+    <row r="3" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="25">
         <f>Questionnaire!C9+Questionnaire!C25+Questionnaire!C32+Questionnaire!C45+Questionnaire!C56+Questionnaire!C63+Questionnaire!C78</f>
         <v>0</v>
       </c>
@@ -2162,13 +2329,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="25"/>
+    <row r="5" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B5" s="26"/>
       <c r="C5" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="str">
         <f>IF(B4&gt;=16,"Rôle favori",IF(B4&gt;=10,"Rôle classique",IF(B4&gt;=6,"Rôle mineur",IF(B4&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2177,9 +2344,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="24">
+    <row r="7" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="25">
         <f>Questionnaire!C15+Questionnaire!C22+Questionnaire!C36+Questionnaire!C43+Questionnaire!C51+Questionnaire!C67+Questionnaire!C74</f>
         <v>0</v>
       </c>
@@ -2187,13 +2354,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
+    <row r="9" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="26"/>
       <c r="C9" s="18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="str">
         <f>IF(B8&gt;=16,"Rôle favori",IF(B8&gt;=10,"Rôle classique",IF(B8&gt;=6,"Rôle mineur",IF(B8&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2202,9 +2369,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="24">
+    <row r="11" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="25">
         <f>Questionnaire!C12+Questionnaire!C20+Questionnaire!C34+Questionnaire!C41+Questionnaire!C59+Questionnaire!C62+Questionnaire!C80</f>
         <v>0</v>
       </c>
@@ -2212,13 +2379,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
+    <row r="13" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="26"/>
       <c r="C13" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="str">
         <f>IF(B12&gt;=16,"Rôle favori",IF(B12&gt;=10,"Rôle classique",IF(B12&gt;=6,"Rôle mineur",IF(B12&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2227,9 +2394,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="24">
+    <row r="15" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="25">
         <f>Questionnaire!C14+Questionnaire!C18+Questionnaire!C37+Questionnaire!C44+Questionnaire!C52+Questionnaire!C68+Questionnaire!C77</f>
         <v>0</v>
       </c>
@@ -2237,13 +2404,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
+    <row r="17" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="26"/>
       <c r="C17" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="str">
         <f>IF(B16&gt;=16,"Rôle favori",IF(B16&gt;=10,"Rôle classique",IF(B16&gt;=6,"Rôle mineur",IF(B16&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2252,9 +2419,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="24">
+    <row r="19" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="25">
         <f>Questionnaire!C13+Questionnaire!C23+Questionnaire!C31+Questionnaire!C42+Questionnaire!C54+Questionnaire!C69+Questionnaire!C73</f>
         <v>0</v>
       </c>
@@ -2262,13 +2429,13 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
+    <row r="21" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B21" s="26"/>
       <c r="C21" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="str">
         <f>IF(B20&gt;=16,"Rôle favori",IF(B20&gt;=10,"Rôle classique",IF(B20&gt;=6,"Rôle mineur",IF(B20&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2277,9 +2444,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="24">
+    <row r="23" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="25">
         <f>Questionnaire!C11+Questionnaire!C26+Questionnaire!C30+Questionnaire!C46+Questionnaire!C57+Questionnaire!C66+Questionnaire!C75</f>
         <v>0</v>
       </c>
@@ -2287,13 +2454,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
+    <row r="25" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="26"/>
       <c r="C25" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="str">
         <f>IF(B24&gt;=16,"Rôle favori",IF(B24&gt;=10,"Rôle classique",IF(B24&gt;=6,"Rôle mineur",IF(B24&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2302,9 +2469,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="24">
+    <row r="27" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="25">
         <f>Questionnaire!C10+Questionnaire!C19+Questionnaire!C29+Questionnaire!C48+Questionnaire!C58+Questionnaire!C65+Questionnaire!C79</f>
         <v>0</v>
       </c>
@@ -2312,13 +2479,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
+    <row r="29" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B29" s="26"/>
       <c r="C29" s="18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="str">
         <f>IF(B28&gt;=16,"Rôle favori",IF(B28&gt;=10,"Rôle classique",IF(B28&gt;=6,"Rôle mineur",IF(B28&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2327,9 +2494,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="24">
+    <row r="31" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="25">
         <f>Questionnaire!C7+Questionnaire!C21+Questionnaire!C35+Questionnaire!C47+Questionnaire!C55+Questionnaire!C70+Questionnaire!C76</f>
         <v>0</v>
       </c>
@@ -2337,13 +2504,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
+    <row r="33" spans="2:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="B33" s="26"/>
       <c r="C33" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="str">
         <f>IF(B32&gt;=16,"Rôle favori",IF(B32&gt;=10,"Rôle classique",IF(B32&gt;=6,"Rôle mineur",IF(B32&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2352,9 +2519,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="24">
+    <row r="35" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="25">
         <f>Questionnaire!C8+Questionnaire!C24+Questionnaire!C33+Questionnaire!C40+Questionnaire!C53+Questionnaire!C64+Questionnaire!C81</f>
         <v>0</v>
       </c>
@@ -2362,13 +2529,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
+    <row r="37" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B37" s="26"/>
       <c r="C37" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="str">
         <f>IF(B36&gt;=16,"Rôle favori",IF(B36&gt;=10,"Rôle classique",IF(B36&gt;=6,"Rôle mineur",IF(B36&gt;=0,"Rôle complexe","false"))))</f>
         <v>Rôle complexe</v>
@@ -2377,12 +2544,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="21" t="s">
         <v>125</v>
       </c>
@@ -2390,7 +2557,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="21" t="s">
         <v>120</v>
       </c>
@@ -2398,7 +2565,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="21" t="s">
         <v>122</v>
       </c>
@@ -2406,7 +2573,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="21" t="s">
         <v>124</v>
       </c>
@@ -2427,5 +2594,6 @@
     <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>